<commit_message>
MAJ Gantt et Ajout au Git
</commit_message>
<xml_diff>
--- a/06_Plateforme_Bron/nomenclature_kit_de_montage.xlsx
+++ b/06_Plateforme_Bron/nomenclature_kit_de_montage.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="11">
   <si>
     <t>Kit :</t>
   </si>
@@ -222,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -257,17 +257,6 @@
       </right>
       <top/>
       <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -409,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,37 +406,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,15 +452,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -782,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,52 +786,52 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="25" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="19.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="21" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -852,14 +840,14 @@
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="21" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -868,14 +856,14 @@
       <c r="B9" s="5"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="21" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -884,14 +872,14 @@
       <c r="B10" s="5"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="21" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -900,14 +888,14 @@
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="21" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -916,14 +904,14 @@
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="21" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -932,14 +920,14 @@
       <c r="B13" s="5"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="21" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -948,14 +936,14 @@
       <c r="B14" s="5"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="21" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -964,14 +952,14 @@
       <c r="B15" s="5"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="21" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -980,14 +968,14 @@
       <c r="B16" s="5"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="21" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -996,14 +984,14 @@
       <c r="B17" s="5"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="21" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1012,14 +1000,14 @@
       <c r="B18" s="5"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="21" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1028,14 +1016,14 @@
       <c r="B19" s="5"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="21" t="s">
+      <c r="E19" s="9"/>
+      <c r="F19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1044,14 +1032,14 @@
       <c r="B20" s="5"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="21" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1060,14 +1048,14 @@
       <c r="B21" s="5"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="21" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1076,14 +1064,14 @@
       <c r="B22" s="5"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="21" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1092,14 +1080,14 @@
       <c r="B23" s="5"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="21" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1108,14 +1096,14 @@
       <c r="B24" s="5"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="21" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1124,14 +1112,14 @@
       <c r="B25" s="5"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="21" t="s">
+      <c r="E25" s="9"/>
+      <c r="F25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1140,14 +1128,14 @@
       <c r="B26" s="5"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="21" t="s">
+      <c r="E26" s="9"/>
+      <c r="F26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1156,14 +1144,14 @@
       <c r="B27" s="5"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="21" t="s">
+      <c r="E27" s="9"/>
+      <c r="F27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1172,14 +1160,14 @@
       <c r="B28" s="5"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="21" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1188,13 +1176,13 @@
       <c r="B29" s="6"/>
       <c r="C29" s="4"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="21" t="s">
+      <c r="F29" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1217,56 +1205,80 @@
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" ht="19.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="29" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F32" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" ht="19.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+    </row>
+    <row r="33" spans="1:8" ht="19.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="19.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E34" s="9"/>
+      <c r="F34" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="19.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E35" s="9"/>
+      <c r="F35" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>

</xml_diff>